<commit_message>
a caminho de Twa Dwet
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -19,10 +19,10 @@
     <t>Dia</t>
   </si>
   <si>
-    <t>Total Palavras</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>Diferença</t>
+    <t>Diff</t>
   </si>
 </sst>
 </file>
@@ -89,13 +89,903 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>42287</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42288</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42289</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42290</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42291</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42293</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42294</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42295</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42296</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42297</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42299</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42301</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42303</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42305</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42306</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42307</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42308</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42309</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>42529</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43528</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44322</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44763</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="197099928"/>
+        <c:axId val="197100320"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="197099928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-816]d/mmm;@" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="197100320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="197100320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="197099928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38098</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C24" totalsRowShown="0">
+  <autoFilter ref="A1:C24"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Dia" dataDxfId="2"/>
-    <tableColumn id="2" name="Total Palavras" dataDxfId="1"/>
-    <tableColumn id="3" name="Diferença" dataDxfId="0">
+    <tableColumn id="2" name="Total" dataDxfId="1"/>
+    <tableColumn id="3" name="Diff" dataDxfId="0">
       <calculatedColumnFormula>B2-B1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -390,17 +1280,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -416,7 +1305,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42262</v>
+        <v>42287</v>
       </c>
       <c r="B2" s="2">
         <v>42529</v>
@@ -426,87 +1315,238 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="1">
+        <v>42288</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43528</v>
+      </c>
       <c r="C3" s="2">
         <f>B3-B2</f>
-        <v>-42529</v>
+        <v>999</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="1">
+        <v>42289</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43928</v>
+      </c>
+      <c r="C4" s="2">
+        <f>B4-B3</f>
+        <v>400</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="1">
+        <v>42290</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44322</v>
+      </c>
+      <c r="C5" s="2">
+        <f>B5-B4</f>
+        <v>394</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="1">
+        <v>42291</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44763</v>
+      </c>
+      <c r="C6" s="2">
+        <f>B6-B5</f>
+        <v>441</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>42292</v>
+      </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C24" si="0">B7-B6</f>
+        <v>-44763</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>42293</v>
+      </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>42294</v>
+      </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>42295</v>
+      </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>42296</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1">
+        <v>42297</v>
+      </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>42298</v>
+      </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>42299</v>
+      </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>42300</v>
+      </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>42301</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>42302</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42303</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>42304</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42305</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42306</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>42307</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>42308</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chegada à entrada de Twa Dwet
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Dia</t>
   </si>
@@ -24,12 +24,15 @@
   <si>
     <t>Diff</t>
   </si>
+  <si>
+    <t>Goal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,13 +40,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -58,15 +74,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -149,10 +169,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>42287</c:v>
                 </c:pt>
@@ -221,16 +241,28 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>42309</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42310</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42311</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42312</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>42313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$24</c:f>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>42529</c:v>
                 </c:pt>
@@ -245,6 +277,148 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>44763</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44763</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44763</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46506</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>42529</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43029</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43529</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45029</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45529</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46029</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46529</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47029</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47529</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48029</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48529</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49029</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>49529</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50529</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>51029</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>51529</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>52529</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>53029</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53529</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>54029</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>54529</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>55029</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>55529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -261,11 +435,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197099928"/>
-        <c:axId val="197100320"/>
+        <c:axId val="194969448"/>
+        <c:axId val="194969840"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="197099928"/>
+        <c:axId val="194969448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -308,16 +482,17 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197100320"/>
+        <c:crossAx val="194969840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="197100320"/>
+        <c:axId val="194969840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="42000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -352,9 +527,10 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197099928"/>
+        <c:crossAx val="194969448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -949,15 +1125,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>38098</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:colOff>9523</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -980,13 +1156,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C24" totalsRowShown="0">
-  <autoFilter ref="A1:C24"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Dia" dataDxfId="2"/>
-    <tableColumn id="2" name="Total" dataDxfId="1"/>
-    <tableColumn id="3" name="Diff" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D28" totalsRowShown="0">
+  <autoFilter ref="A1:D28"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Dia" dataDxfId="3"/>
+    <tableColumn id="2" name="Total" dataDxfId="2"/>
+    <tableColumn id="3" name="Diff" dataDxfId="1">
       <calculatedColumnFormula>B2-B1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Goal" dataDxfId="0">
+      <calculatedColumnFormula>D1+$C$2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1280,10 +1459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,7 +1471,7 @@
     <col min="2" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1302,19 +1481,26 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42287</v>
       </c>
       <c r="B2" s="2">
         <v>42529</v>
       </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <v>500</v>
+      </c>
+      <c r="D2" s="2">
+        <f>Table1[[#This Row],[Total]]</f>
+        <v>42529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42288</v>
       </c>
@@ -1322,11 +1508,15 @@
         <v>43528</v>
       </c>
       <c r="C3" s="2">
-        <f>B3-B2</f>
+        <f t="shared" ref="C3:C24" si="0">B3-B2</f>
         <v>999</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D24" si="1">D2+$C$2</f>
+        <v>43029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42289</v>
       </c>
@@ -1334,11 +1524,15 @@
         <v>43928</v>
       </c>
       <c r="C4" s="2">
-        <f>B4-B3</f>
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>43529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42290</v>
       </c>
@@ -1346,11 +1540,15 @@
         <v>44322</v>
       </c>
       <c r="C5" s="2">
-        <f>B5-B4</f>
+        <f t="shared" si="0"/>
         <v>394</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>44029</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42291</v>
       </c>
@@ -1358,61 +1556,93 @@
         <v>44763</v>
       </c>
       <c r="C6" s="2">
-        <f>B6-B5</f>
+        <f t="shared" si="0"/>
         <v>441</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>44529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42292</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>44763</v>
+      </c>
       <c r="C7" s="2">
-        <f t="shared" ref="C7:C24" si="0">B7-B6</f>
-        <v>-44763</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>45029</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42293</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>44763</v>
+      </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42294</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>45976</v>
+      </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1213</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>46029</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42295</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>46506</v>
+      </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>46529</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42296</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-46506</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>47029</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42297</v>
       </c>
@@ -1421,8 +1651,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>47529</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42298</v>
       </c>
@@ -1431,8 +1665,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="1"/>
+        <v>48029</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42299</v>
       </c>
@@ -1441,8 +1679,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>48529</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42300</v>
       </c>
@@ -1451,8 +1693,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>49029</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42301</v>
       </c>
@@ -1461,8 +1707,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <f t="shared" si="1"/>
+        <v>49529</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42302</v>
       </c>
@@ -1471,8 +1721,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>50029</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42303</v>
       </c>
@@ -1481,8 +1735,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" si="1"/>
+        <v>50529</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42304</v>
       </c>
@@ -1491,8 +1749,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="1"/>
+        <v>51029</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42305</v>
       </c>
@@ -1501,8 +1763,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <f t="shared" si="1"/>
+        <v>51529</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42306</v>
       </c>
@@ -1511,8 +1777,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <f t="shared" si="1"/>
+        <v>52029</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42307</v>
       </c>
@@ -1521,8 +1791,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
+        <v>52529</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42308</v>
       </c>
@@ -1531,8 +1805,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <f t="shared" si="1"/>
+        <v>53029</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42309</v>
       </c>
@@ -1541,12 +1819,73 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D24" s="2">
+        <f t="shared" si="1"/>
+        <v>53529</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2">
+        <f t="shared" ref="C25:C28" si="2">B25-B24</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" ref="D25:D28" si="3">D24+$C$2</f>
+        <v>54029</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="3"/>
+        <v>54529</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>42312</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="3"/>
+        <v>55029</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>42313</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="3"/>
+        <v>55529</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fim capitulo 9 (chegada Twa Dwet)
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -290,6 +290,9 @@
                 <c:pt idx="8">
                   <c:v>46506</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>46818</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -435,11 +438,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="194969448"/>
-        <c:axId val="194969840"/>
+        <c:axId val="196983048"/>
+        <c:axId val="196981088"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="194969448"/>
+        <c:axId val="196983048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,14 +485,14 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194969840"/>
+        <c:crossAx val="196981088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="194969840"/>
+        <c:axId val="196981088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42000"/>
@@ -527,7 +530,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194969448"/>
+        <c:crossAx val="196983048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -1461,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,10 +1635,12 @@
       <c r="A11" s="1">
         <v>42296</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>46818</v>
+      </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>-46506</v>
+        <v>312</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
@@ -1649,7 +1654,7 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-46818</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
more words for NaNoWriMo
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,7 +83,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -110,7 +122,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -169,10 +181,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$28</c:f>
+              <c:f>Sheet1!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>42287</c:v>
                 </c:pt>
@@ -253,16 +265,28 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>42313</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>42314</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>42315</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42316</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42317</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:f>Sheet1!$B$2:$B$83</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>42529</c:v>
                 </c:pt>
@@ -292,11 +316,61 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>46818</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46818</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46818</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46818</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47253</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47502</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48843</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>49118</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49118</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>49439</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49439</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>49439</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>49439</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>50028</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>50306</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50750</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7CF4-4DA0-A8E7-238C2A9E0B8C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -338,95 +412,112 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$28</c:f>
+              <c:f>Sheet1!$D$2:$D$83</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>42529</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43029</c:v>
+                  <c:v>42929</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43529</c:v>
+                  <c:v>43329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44029</c:v>
+                  <c:v>43729</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>44129</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>44529</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>45029</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>45529</c:v>
+                  <c:v>44929</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46029</c:v>
+                  <c:v>45329</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>45729</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46129</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>46529</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>47029</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>47529</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>48029</c:v>
+                  <c:v>46929</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>47329</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47729</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48129</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>48529</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>49029</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49529</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>50029</c:v>
-                </c:pt>
                 <c:pt idx="16">
+                  <c:v>48929</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49329</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>49729</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50129</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>50529</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>51029</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>51529</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>52029</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
+                  <c:v>50929</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>51329</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>51729</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>52129</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>52529</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>53029</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>53529</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>54029</c:v>
-                </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
+                  <c:v>52929</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>53329</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>53729</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>54129</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>54529</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>55029</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>55529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7CF4-4DA0-A8E7-238C2A9E0B8C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1159,15 +1250,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D28" totalsRowShown="0">
-  <autoFilter ref="A1:D28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D33" totalsRowCount="1">
+  <autoFilter ref="A1:D32"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Dia" dataDxfId="3"/>
-    <tableColumn id="2" name="Total" dataDxfId="2"/>
-    <tableColumn id="3" name="Diff" dataDxfId="1">
+    <tableColumn id="1" name="Dia" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="2" name="Total" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="Diff" dataDxfId="5" totalsRowDxfId="1">
       <calculatedColumnFormula>B2-B1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="0">
+    <tableColumn id="5" name="Goal" dataDxfId="4" totalsRowDxfId="0">
       <calculatedColumnFormula>D1+$C$2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1462,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1587,7 @@
         <v>42529</v>
       </c>
       <c r="C2" s="3">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D2" s="2">
         <f>Table1[[#This Row],[Total]]</f>
@@ -1516,7 +1607,7 @@
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D24" si="1">D2+$C$2</f>
-        <v>43029</v>
+        <v>42929</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1532,7 +1623,7 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>43529</v>
+        <v>43329</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1548,7 +1639,7 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>44029</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,7 +1655,7 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>44529</v>
+        <v>44129</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1580,7 +1671,7 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>45029</v>
+        <v>44529</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1596,7 +1687,7 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>45529</v>
+        <v>44929</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1612,7 +1703,7 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>46029</v>
+        <v>45329</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1628,7 +1719,7 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>46529</v>
+        <v>45729</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,217 +1735,247 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>47029</v>
+        <v>46129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42297</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>46818</v>
+      </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>-46818</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>47529</v>
+        <v>46529</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42298</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>46818</v>
+      </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>48029</v>
+        <v>46929</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42299</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>46818</v>
+      </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>48529</v>
+        <v>47329</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42300</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>47253</v>
+      </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>435</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>49029</v>
+        <v>47729</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42301</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>47502</v>
+      </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>49529</v>
+        <v>48129</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42302</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>48843</v>
+      </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1341</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>50029</v>
+        <v>48529</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42303</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>49118</v>
+      </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>50529</v>
+        <v>48929</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42304</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>49118</v>
+      </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>51029</v>
+        <v>49329</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42305</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>49439</v>
+      </c>
       <c r="C20" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>321</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>51529</v>
+        <v>49729</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42306</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>49439</v>
+      </c>
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>52029</v>
+        <v>50129</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42307</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>49439</v>
+      </c>
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>52529</v>
+        <v>50529</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42308</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2">
+        <v>49439</v>
+      </c>
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>53029</v>
+        <v>50929</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42309</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2">
+        <v>50028</v>
+      </c>
       <c r="C24" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>589</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>53529</v>
+        <v>51329</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42310</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>50306</v>
+      </c>
       <c r="C25" s="2">
         <f t="shared" ref="C25:C28" si="2">B25-B24</f>
-        <v>0</v>
+        <v>278</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" ref="D25:D28" si="3">D24+$C$2</f>
-        <v>54029</v>
+        <v>51729</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42311</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>50750</v>
+      </c>
       <c r="C26" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>444</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="3"/>
-        <v>54529</v>
+        <v>52129</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,11 +1985,11 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-50750</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="3"/>
-        <v>55029</v>
+        <v>52529</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1882,8 +2003,70 @@
       </c>
       <c r="D28" s="2">
         <f t="shared" si="3"/>
-        <v>55529</v>
-      </c>
+        <v>52929</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>42314</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2">
+        <f t="shared" ref="C29:C32" si="4">B29-B28</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" ref="D29:D32" si="5">D28+$C$2</f>
+        <v>53329</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>42315</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="5"/>
+        <v>53729</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>42316</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="5"/>
+        <v>54129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="5"/>
+        <v>54529</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
quase terminado cap 10
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -137,7 +137,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.5693247009889631E-2"/>
+          <c:y val="1.9622269762020493E-2"/>
+          <c:w val="0.87231201101287303"/>
+          <c:h val="0.9328952365472345"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -181,10 +191,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$83</c:f>
+              <c:f>Sheet1!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="82"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>42287</c:v>
                 </c:pt>
@@ -261,32 +271,53 @@
                   <c:v>42311</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42312</c:v>
+                  <c:v>42342</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42313</c:v>
+                  <c:v>42343</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42314</c:v>
+                  <c:v>42344</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42315</c:v>
+                  <c:v>42345</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42316</c:v>
+                  <c:v>42346</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42317</c:v>
+                  <c:v>42347</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42348</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42349</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42350</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42351</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42352</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42353</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42354</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$83</c:f>
+              <c:f>Sheet1!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="82"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>42529</c:v>
                 </c:pt>
@@ -361,6 +392,45 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>50750</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>50750</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>50750</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>50750</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>50750</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>50750</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50870</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>50870</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>50991</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>51286</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>51473</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>51473</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>51473</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>51473</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -410,6 +480,129 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$39</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>42287</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42288</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42289</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42290</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42291</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42293</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42294</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42295</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42296</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42297</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42299</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42301</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42303</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42305</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42306</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42307</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42308</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42309</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42310</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42311</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42342</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>42343</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>42344</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>42345</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42346</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42347</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42348</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42349</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42350</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42351</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42352</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42353</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$83</c:f>
@@ -508,6 +701,27 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>54529</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>54929</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>55329</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>55729</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>56129</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>56529</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>56929</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>57329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -635,7 +849,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1218,16 +1432,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9523</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1250,8 +1464,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D33" totalsRowCount="1">
-  <autoFilter ref="A1:D32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D40" totalsRowCount="1">
+  <autoFilter ref="A1:D39"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Dia" dataDxfId="7" totalsRowDxfId="3"/>
     <tableColumn id="2" name="Total" dataDxfId="6" totalsRowDxfId="2"/>
@@ -1553,10 +1767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,12 +2194,14 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>42312</v>
-      </c>
-      <c r="B27" s="2"/>
+        <v>42342</v>
+      </c>
+      <c r="B27" s="2">
+        <v>50750</v>
+      </c>
       <c r="C27" s="2">
         <f t="shared" si="2"/>
-        <v>-50750</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="3"/>
@@ -1994,9 +2210,11 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>42313</v>
-      </c>
-      <c r="B28" s="2"/>
+        <v>42343</v>
+      </c>
+      <c r="B28" s="2">
+        <v>50750</v>
+      </c>
       <c r="C28" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2008,9 +2226,11 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>42314</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>42344</v>
+      </c>
+      <c r="B29" s="2">
+        <v>50750</v>
+      </c>
       <c r="C29" s="2">
         <f t="shared" ref="C29:C32" si="4">B29-B28</f>
         <v>0</v>
@@ -2022,9 +2242,11 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>42315</v>
-      </c>
-      <c r="B30" s="2"/>
+        <v>42345</v>
+      </c>
+      <c r="B30" s="2">
+        <v>50750</v>
+      </c>
       <c r="C30" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2036,9 +2258,11 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>42316</v>
-      </c>
-      <c r="B31" s="2"/>
+        <v>42346</v>
+      </c>
+      <c r="B31" s="2">
+        <v>50750</v>
+      </c>
       <c r="C31" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2050,12 +2274,14 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>42317</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>42347</v>
+      </c>
+      <c r="B32" s="2">
+        <v>50870</v>
+      </c>
       <c r="C32" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" si="5"/>
@@ -2063,10 +2289,122 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="A33" s="1">
+        <v>42348</v>
+      </c>
+      <c r="B33" s="2">
+        <v>50870</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" ref="C33:C39" si="6">B33-B32</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" ref="D33:D39" si="7">D32+$C$2</f>
+        <v>54929</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>42349</v>
+      </c>
+      <c r="B34" s="2">
+        <v>50991</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="6"/>
+        <v>121</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="7"/>
+        <v>55329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>42350</v>
+      </c>
+      <c r="B35" s="2">
+        <v>51286</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="6"/>
+        <v>295</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="7"/>
+        <v>55729</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>42351</v>
+      </c>
+      <c r="B36" s="2">
+        <v>51473</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="6"/>
+        <v>187</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="7"/>
+        <v>56129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>42352</v>
+      </c>
+      <c r="B37" s="2">
+        <v>51473</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="7"/>
+        <v>56529</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>42353</v>
+      </c>
+      <c r="B38" s="2">
+        <v>51473</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="7"/>
+        <v>56929</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>42354</v>
+      </c>
+      <c r="B39" s="2">
+        <v>51473</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="7"/>
+        <v>57329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fim cap 10 (à pressa)
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -191,10 +191,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$39</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>42287</c:v>
                 </c:pt>
@@ -308,16 +308,25 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>42354</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42355</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42356</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$39</c:f>
+              <c:f>Sheet1!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>42529</c:v>
                 </c:pt>
@@ -431,6 +440,15 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>51473</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>51473</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>51473</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>51514</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -482,10 +500,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$39</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>42287</c:v>
                 </c:pt>
@@ -599,6 +617,15 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>42354</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42355</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42356</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,6 +749,15 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>57329</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>57729</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>58129</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>58529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1464,8 +1500,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D40" totalsRowCount="1">
-  <autoFilter ref="A1:D39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D43" totalsRowCount="1">
+  <autoFilter ref="A1:D42"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Dia" dataDxfId="7" totalsRowDxfId="3"/>
     <tableColumn id="2" name="Total" dataDxfId="6" totalsRowDxfId="2"/>
@@ -1767,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,10 +2437,58 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="A40" s="1">
+        <v>42355</v>
+      </c>
+      <c r="B40" s="2">
+        <v>51473</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" ref="C40:C42" si="8">B40-B39</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" ref="D40:D42" si="9">D39+$C$2</f>
+        <v>57729</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42356</v>
+      </c>
+      <c r="B41" s="2">
+        <v>51473</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="9"/>
+        <v>58129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>42357</v>
+      </c>
+      <c r="B42" s="2">
+        <v>51514</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="8"/>
+        <v>41</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="9"/>
+        <v>58529</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>